<commit_message>
tested app flashing and jump to app
</commit_message>
<xml_diff>
--- a/doc/Bootloader_commands.xlsx
+++ b/doc/Bootloader_commands.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="commands" sheetId="1" r:id="rId1"/>
@@ -186,40 +186,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,343 +515,343 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="2:13" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="2:13" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="7"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="7"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="7"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="7"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="7"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="7"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="7"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="7"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -879,7 +879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
@@ -894,54 +894,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="5" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="P7" s="2" t="s">
+      <c r="P7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.3">
       <c r="K8" s="1" t="s">
@@ -950,42 +950,42 @@
       <c r="L8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="14" t="s">
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
     </row>
     <row r="9" spans="3:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
     </row>
     <row r="10" spans="3:19" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L10" s="12"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.3">
       <c r="L14" t="s">

</xml_diff>